<commit_message>
protected routing search includes
</commit_message>
<xml_diff>
--- a/leetcode/Sep_leetcodetracker.xlsx
+++ b/leetcode/Sep_leetcodetracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakshisrivastava/Desktop/hanumant_fullstack/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84C76F3-4A65-FC44-B01C-3BB397D4961C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00F8D61-3217-8745-BFB7-9FDA0858949D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="15560" xr2:uid="{7223D205-73F4-4148-BF4C-16C1EFE483E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="127">
   <si>
     <t>Sakshi neetcode Track</t>
   </si>
@@ -365,9 +365,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>5 questions a day</t>
-  </si>
-  <si>
     <t>SIT FOR 10 HOUS AND STUDY---BOYCOTT EVERYTHING</t>
   </si>
   <si>
@@ -387,6 +384,39 @@
   </si>
   <si>
     <t>1:14pm</t>
+  </si>
+  <si>
+    <t>6:31pm</t>
+  </si>
+  <si>
+    <t>12 days</t>
+  </si>
+  <si>
+    <t>5:36am</t>
+  </si>
+  <si>
+    <t>6:07pm</t>
+  </si>
+  <si>
+    <t>6:28pm</t>
+  </si>
+  <si>
+    <t>25th-Sep</t>
+  </si>
+  <si>
+    <t>7:14AM</t>
+  </si>
+  <si>
+    <t>8:07am</t>
+  </si>
+  <si>
+    <t>8:47am</t>
+  </si>
+  <si>
+    <t>10 days</t>
+  </si>
+  <si>
+    <t>1 greedy , 6 interval pending</t>
   </si>
 </sst>
 </file>
@@ -935,7 +965,7 @@
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1522,10 +1552,10 @@
       </c>
       <c r="G25" s="17"/>
       <c r="N25" t="s">
+        <v>110</v>
+      </c>
+      <c r="O25" t="s">
         <v>111</v>
-      </c>
-      <c r="O25" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
@@ -1533,42 +1563,75 @@
         <v>45558</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="D26" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="E26" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="F26" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F26" s="6"/>
-      <c r="G26" s="17"/>
-      <c r="I26" s="10" t="s">
-        <v>110</v>
+      <c r="G26" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26" s="10">
+        <v>34</v>
+      </c>
+      <c r="M26" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
+      <c r="A27" s="3">
+        <v>45559</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>118</v>
+      </c>
       <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
+      <c r="D27" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>120</v>
+      </c>
       <c r="F27" s="6"/>
       <c r="G27" s="17"/>
+      <c r="O27" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A28" s="3"/>
+      <c r="A28" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="B28" s="3"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
+        <v>122</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>124</v>
+      </c>
       <c r="G28" s="17"/>
+      <c r="I28" s="10">
+        <v>29</v>
+      </c>
+      <c r="M28" t="s">
+        <v>125</v>
+      </c>
+      <c r="N28" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>

</xml_diff>

<commit_message>
reducer action state dispatch
</commit_message>
<xml_diff>
--- a/leetcode/Sep_leetcodetracker.xlsx
+++ b/leetcode/Sep_leetcodetracker.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakshisrivastava/Desktop/hanumant_fullstack/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00F8D61-3217-8745-BFB7-9FDA0858949D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C287F04-766A-6541-A991-0F2052BC1563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="15560" xr2:uid="{7223D205-73F4-4148-BF4C-16C1EFE483E0}"/>
   </bookViews>
   <sheets>
     <sheet name="neetcode 150 Tracker" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="137">
   <si>
     <t>Sakshi neetcode Track</t>
   </si>
@@ -401,9 +402,6 @@
     <t>6:28pm</t>
   </si>
   <si>
-    <t>25th-Sep</t>
-  </si>
-  <si>
     <t>7:14AM</t>
   </si>
   <si>
@@ -416,14 +414,314 @@
     <t>10 days</t>
   </si>
   <si>
-    <t>1 greedy , 6 interval pending</t>
+    <t>6:54pm</t>
+  </si>
+  <si>
+    <t>greedy over , 6 interval pending</t>
+  </si>
+  <si>
+    <t>11:36am</t>
+  </si>
+  <si>
+    <t>12:27pm</t>
+  </si>
+  <si>
+    <t>#drawing in a number line intervals is import in interval questions</t>
+  </si>
+  <si>
+    <t># always think of sorting before merign in inteval questions</t>
+  </si>
+  <si>
+    <t>#sort by starting index</t>
+  </si>
+  <si>
+    <r>
+      <t>class</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Solution</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>def</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> merge</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>self</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> intervals</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> List</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>List</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>]])</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> -&gt; List</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>List</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>]]:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>intervals.sort</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>key=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>lambda</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> pair</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>pair</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>])</t>
+    </r>
+  </si>
+  <si>
+    <t>1:04pm</t>
+  </si>
+  <si>
+    <t>4 intervals problem pending</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -451,6 +749,36 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="17"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="17"/>
+      <color rgb="FF608B4E"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="17"/>
+      <color rgb="FF569CD6"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="17"/>
+      <color rgb="FFDCDCDC"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="17"/>
+      <color rgb="FFB5CEA8"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -551,7 +879,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -615,13 +943,14 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="20" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -962,10 +1291,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB9B0579-A1A3-6345-8471-7145320CE37A}">
-  <dimension ref="A1:P37"/>
+  <dimension ref="A1:P38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -992,7 +1321,7 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="27"/>
+      <c r="B2" s="25"/>
       <c r="E2" t="s">
         <v>4</v>
       </c>
@@ -1355,7 +1684,7 @@
       <c r="G18" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H18" s="25" t="s">
+      <c r="H18" s="11" t="s">
         <v>67</v>
       </c>
       <c r="I18" s="10">
@@ -1387,6 +1716,7 @@
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
       <c r="G19" s="17"/>
+      <c r="H19" s="11"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
@@ -1406,7 +1736,7 @@
       <c r="G20" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H20" s="26" t="s">
+      <c r="H20" s="11" t="s">
         <v>81</v>
       </c>
       <c r="I20" s="10">
@@ -1440,7 +1770,7 @@
       <c r="G21" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H21" s="26" t="s">
+      <c r="H21" s="11" t="s">
         <v>85</v>
       </c>
       <c r="I21" s="10">
@@ -1473,6 +1803,7 @@
       <c r="G22" s="17" t="s">
         <v>10</v>
       </c>
+      <c r="H22" s="11"/>
       <c r="I22" s="10">
         <v>46</v>
       </c>
@@ -1497,11 +1828,11 @@
       <c r="E23" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="F23" s="28" t="s">
+      <c r="F23" s="26" t="s">
         <v>100</v>
       </c>
       <c r="G23" s="17"/>
-      <c r="H23" s="25" t="s">
+      <c r="H23" s="11" t="s">
         <v>82</v>
       </c>
       <c r="M23" t="s">
@@ -1529,6 +1860,7 @@
       <c r="G24" s="17" t="s">
         <v>10</v>
       </c>
+      <c r="H24" s="11"/>
       <c r="I24" s="10">
         <v>38</v>
       </c>
@@ -1551,6 +1883,7 @@
         <v>107</v>
       </c>
       <c r="G25" s="17"/>
+      <c r="H25" s="11"/>
       <c r="N25" t="s">
         <v>110</v>
       </c>
@@ -1580,6 +1913,7 @@
       <c r="G26" s="17" t="s">
         <v>10</v>
       </c>
+      <c r="H26" s="11"/>
       <c r="I26" s="10">
         <v>34</v>
       </c>
@@ -1603,52 +1937,69 @@
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="17"/>
+      <c r="H27" s="11"/>
       <c r="O27" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>121</v>
+      <c r="A28" s="3">
+        <v>45560</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="F28" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="G28" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="I28" s="10">
+        <v>28</v>
+      </c>
+      <c r="M28" t="s">
         <v>124</v>
-      </c>
-      <c r="G28" s="17"/>
-      <c r="I28" s="10">
-        <v>29</v>
-      </c>
-      <c r="M28" t="s">
-        <v>125</v>
       </c>
       <c r="N28" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
+      <c r="A29" s="3">
+        <v>45561</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>135</v>
+      </c>
       <c r="F29" s="6"/>
       <c r="G29" s="17"/>
+      <c r="H29" s="11"/>
+      <c r="N29" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="6"/>
-      <c r="D30" s="6" t="s">
-        <v>28</v>
-      </c>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
       <c r="G30" s="17"/>
@@ -1660,9 +2011,6 @@
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="6"/>
-      <c r="D31" s="6" t="s">
-        <v>29</v>
-      </c>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
       <c r="G31" s="17"/>
@@ -1702,7 +2050,7 @@
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
       <c r="G35" s="17"/>
-      <c r="N35" s="29" t="s">
+      <c r="N35" s="27" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1723,6 +2071,14 @@
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="17"/>
+      <c r="N37" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N38" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1730,4 +2086,49 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B735FA6-CBB3-3946-B93E-0EA3535BAD07}">
+  <dimension ref="B15:B20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="15" spans="2:2" ht="22" x14ac:dyDescent="0.25">
+      <c r="B15" s="28" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" ht="22" x14ac:dyDescent="0.25">
+      <c r="B16" s="28" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="22" x14ac:dyDescent="0.25">
+      <c r="B17" s="28" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="22" x14ac:dyDescent="0.25">
+      <c r="B18" s="29" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="22" x14ac:dyDescent="0.25">
+      <c r="B19" s="29" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" ht="22" x14ac:dyDescent="0.25">
+      <c r="B20" s="30" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>